<commit_message>
transposed and adls file read added
</commit_message>
<xml_diff>
--- a/datf_core/test/testprotocol/traversedtestprotocol.xlsx
+++ b/datf_core/test/testprotocol/traversedtestprotocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\DATF_Other\Pyspark\QE_ATF\datf_core\test\testprotocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737E1DA4-CFF9-4E6D-A320-7EA816E698F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D4A7DB-3418-489E-94C8-B4BCB2F9E757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="protocoltestcasedetails" sheetId="2" r:id="rId2"/>
     <sheet name="config" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">protocoltestcasedetails!$A$1:$AI$31</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="177">
   <si>
     <t>Sno.</t>
   </si>
@@ -364,9 +367,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>adls-gen2</t>
-  </si>
-  <si>
     <t>start_date, end_date,operation_type,description</t>
   </si>
   <si>
@@ -560,6 +560,18 @@
   </si>
   <si>
     <t>test/s2t/s2t_30_csv_csv_3mill50cols.xlsx</t>
+  </si>
+  <si>
+    <t>adls</t>
+  </si>
+  <si>
+    <t>postgres</t>
+  </si>
+  <si>
+    <t>gcp-gcs</t>
+  </si>
+  <si>
+    <t>teradata</t>
   </si>
 </sst>
 </file>
@@ -611,7 +623,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -654,12 +666,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -699,6 +720,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -737,13 +759,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BAE0998F-A220-496F-A9F2-1D79AF152730}" name="Table1" displayName="Table1" ref="A1:E10" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BAE0998F-A220-496F-A9F2-1D79AF152730}" name="Table1" displayName="Table1" ref="A1:E13" totalsRowShown="0" headerRowDxfId="0">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B7EB12A5-7DBB-4555-B2C0-33C41BB1C784}" name="comparetype"/>
     <tableColumn id="2" xr3:uid="{29FBA9CE-F214-413F-8067-886B551BF267}" name="querygenerationmode"/>
+    <tableColumn id="5" xr3:uid="{D4F645CD-0CC3-41EA-B655-EFEDB67C1620}" name="yesorno"/>
+    <tableColumn id="4" xr3:uid="{3031386E-16DA-44EE-AA9B-4DE756532190}" name="fileformat"/>
     <tableColumn id="3" xr3:uid="{4C653E17-7023-4482-B115-734A3096F5F2}" name="connectiontype"/>
-    <tableColumn id="4" xr3:uid="{3031386E-16DA-44EE-AA9B-4DE756532190}" name="fileformat"/>
-    <tableColumn id="5" xr3:uid="{D4F645CD-0CC3-41EA-B655-EFEDB67C1620}" name="yesorno"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1084,8 +1106,8 @@
   <dimension ref="A1:AI37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,7 +1299,7 @@
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>78</v>
@@ -1330,7 +1352,7 @@
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AG3" s="2" t="s">
         <v>78</v>
@@ -1383,7 +1405,7 @@
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
       <c r="AF4" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AG4" s="2" t="s">
         <v>78</v>
@@ -1436,7 +1458,7 @@
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AG5" s="2" t="s">
         <v>78</v>
@@ -1489,7 +1511,7 @@
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AG6" s="2" t="s">
         <v>78</v>
@@ -1542,7 +1564,7 @@
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG7" s="2" t="s">
         <v>78</v>
@@ -1595,7 +1617,7 @@
       <c r="AD8" s="2"/>
       <c r="AE8" s="2"/>
       <c r="AF8" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AG8" s="2" t="s">
         <v>78</v>
@@ -1648,7 +1670,7 @@
       <c r="AD9" s="2"/>
       <c r="AE9" s="2"/>
       <c r="AF9" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG9" s="2" t="s">
         <v>78</v>
@@ -1701,13 +1723,13 @@
       <c r="AD10" s="2"/>
       <c r="AE10" s="2"/>
       <c r="AF10" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AG10" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AH10" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI10" s="14">
         <v>8</v>
@@ -1756,7 +1778,7 @@
       <c r="AD11" s="2"/>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AG11" s="2" t="s">
         <v>78</v>
@@ -1783,10 +1805,10 @@
         <v>80</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>84</v>
@@ -1795,10 +1817,10 @@
         <v>89</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1808,16 +1830,16 @@
         <v>80</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R12" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S12" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="S12" s="2" t="s">
+      <c r="T12" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="U12" s="2" t="s">
         <v>84</v>
@@ -1826,10 +1848,10 @@
         <v>89</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
@@ -1839,19 +1861,19 @@
         <v>80</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AG12" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AH12" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI12" s="2">
         <v>5</v>
@@ -1868,16 +1890,16 @@
         <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>84</v>
@@ -1886,10 +1908,10 @@
         <v>89</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1899,16 +1921,16 @@
         <v>80</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R13" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S13" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="S13" s="2" t="s">
+      <c r="T13" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="U13" s="2" t="s">
         <v>84</v>
@@ -1917,10 +1939,10 @@
         <v>89</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
@@ -1930,22 +1952,20 @@
         <v>80</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AF13" s="2" t="s">
-        <v>155</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="AF13" s="2"/>
       <c r="AG13" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AH13" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI13" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -1965,10 +1985,10 @@
         <v>80</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>84</v>
@@ -1977,31 +1997,31 @@
         <v>88</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>31</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S14" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="T14" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="U14" s="2" t="s">
         <v>84</v>
@@ -2010,10 +2030,10 @@
         <v>89</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
@@ -2021,19 +2041,19 @@
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AG14" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AH14" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI14" s="2">
         <v>5</v>
@@ -2056,10 +2076,10 @@
         <v>80</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>84</v>
@@ -2068,31 +2088,31 @@
         <v>88</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>31</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S15" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="T15" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="U15" s="2" t="s">
         <v>84</v>
@@ -2101,10 +2121,10 @@
         <v>89</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
@@ -2112,19 +2132,19 @@
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AF15" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG15" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AH15" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI15" s="2">
         <v>5</v>
@@ -2147,10 +2167,10 @@
         <v>77</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>84</v>
@@ -2159,10 +2179,10 @@
         <v>89</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -2172,10 +2192,10 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="U16" s="2" t="s">
         <v>84</v>
@@ -2184,10 +2204,10 @@
         <v>89</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
@@ -2201,7 +2221,7 @@
         <v>78</v>
       </c>
       <c r="AH16" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI16" s="2">
         <v>5</v>
@@ -2224,10 +2244,10 @@
         <v>77</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>84</v>
@@ -2236,10 +2256,10 @@
         <v>89</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -2249,10 +2269,10 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="U17" s="2" t="s">
         <v>84</v>
@@ -2261,10 +2281,10 @@
         <v>89</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
@@ -2278,7 +2298,7 @@
         <v>78</v>
       </c>
       <c r="AH17" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI17" s="2">
         <v>5</v>
@@ -2301,10 +2321,10 @@
         <v>77</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>94</v>
@@ -2313,10 +2333,10 @@
         <v>91</v>
       </c>
       <c r="J18" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -2328,10 +2348,10 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U18" s="2" t="s">
         <v>94</v>
@@ -2340,10 +2360,10 @@
         <v>91</v>
       </c>
       <c r="W18" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="X18" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
@@ -2358,7 +2378,7 @@
         <v>78</v>
       </c>
       <c r="AH18" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI18" s="2">
         <v>5</v>
@@ -2381,10 +2401,10 @@
         <v>77</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>84</v>
@@ -2393,10 +2413,10 @@
         <v>89</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -2408,10 +2428,10 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U19" s="2" t="s">
         <v>94</v>
@@ -2420,10 +2440,10 @@
         <v>91</v>
       </c>
       <c r="W19" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="X19" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="X19" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
@@ -2438,7 +2458,7 @@
         <v>78</v>
       </c>
       <c r="AH19" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI19" s="2">
         <v>5</v>
@@ -2461,10 +2481,10 @@
         <v>77</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>93</v>
@@ -2473,10 +2493,10 @@
         <v>91</v>
       </c>
       <c r="J20" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -2488,10 +2508,10 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U20" s="2" t="s">
         <v>94</v>
@@ -2500,10 +2520,10 @@
         <v>91</v>
       </c>
       <c r="W20" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="X20" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="X20" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
@@ -2514,13 +2534,13 @@
       <c r="AD20" s="2"/>
       <c r="AE20" s="2"/>
       <c r="AF20" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG20" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AH20" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI20" s="14">
         <v>8</v>
@@ -2543,10 +2563,10 @@
         <v>77</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>93</v>
@@ -2555,10 +2575,10 @@
         <v>91</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -2570,10 +2590,10 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="U21" s="2" t="s">
         <v>96</v>
@@ -2582,10 +2602,10 @@
         <v>91</v>
       </c>
       <c r="W21" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="X21" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="X21" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
@@ -2600,7 +2620,7 @@
         <v>78</v>
       </c>
       <c r="AH21" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI21" s="14">
         <v>8</v>
@@ -2623,26 +2643,26 @@
         <v>77</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
         <v>84</v>
       </c>
       <c r="I22" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K22" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="L22" t="s">
         <v>31</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2" t="s">
@@ -2652,10 +2672,10 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="U22" s="2" t="s">
         <v>96</v>
@@ -2664,10 +2684,10 @@
         <v>91</v>
       </c>
       <c r="W22" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="X22" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="X22" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
@@ -2678,13 +2698,13 @@
       <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
       <c r="AF22" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AG22" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AH22" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI22" s="14">
         <v>8</v>
@@ -2707,10 +2727,10 @@
         <v>77</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>96</v>
@@ -2719,10 +2739,10 @@
         <v>91</v>
       </c>
       <c r="J23" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -2734,10 +2754,10 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="U23" s="2" t="s">
         <v>96</v>
@@ -2746,10 +2766,10 @@
         <v>91</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X23" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
@@ -2764,7 +2784,7 @@
         <v>78</v>
       </c>
       <c r="AH23" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI23" s="14">
         <v>5</v>
@@ -2787,10 +2807,10 @@
         <v>77</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>84</v>
@@ -2799,10 +2819,10 @@
         <v>89</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -2814,7 +2834,7 @@
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T24" s="2" t="s">
         <v>102</v>
@@ -2842,7 +2862,7 @@
         <v>78</v>
       </c>
       <c r="AH24" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI24" s="14">
         <v>8</v>
@@ -2942,10 +2962,10 @@
         <v>77</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>93</v>
@@ -2954,27 +2974,27 @@
         <v>91</v>
       </c>
       <c r="J26" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K26" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U26" s="2" t="s">
         <v>93</v>
@@ -2983,10 +3003,10 @@
         <v>91</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="X26" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
@@ -3022,10 +3042,10 @@
         <v>77</v>
       </c>
       <c r="F27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>93</v>
@@ -3034,25 +3054,25 @@
         <v>91</v>
       </c>
       <c r="J27" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U27" s="2" t="s">
         <v>93</v>
@@ -3061,20 +3081,20 @@
         <v>91</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="X27" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
       <c r="AB27" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
       <c r="AF27" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AG27" s="2" t="s">
         <v>78</v>
@@ -3112,7 +3132,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
@@ -3127,19 +3147,19 @@
       <c r="Z28" s="2"/>
       <c r="AA28" s="2"/>
       <c r="AB28" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC28" s="2"/>
       <c r="AD28" s="2"/>
       <c r="AE28" s="2"/>
       <c r="AF28" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AG28" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AH28" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AI28" s="14">
         <v>8</v>
@@ -3162,10 +3182,10 @@
         <v>80</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>93</v>
@@ -3183,16 +3203,16 @@
         <v>80</v>
       </c>
       <c r="Q29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R29" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="S29" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="S29" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="T29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U29" s="2" t="s">
         <v>93</v>
@@ -3210,10 +3230,10 @@
         <v>80</v>
       </c>
       <c r="AD29" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AE29" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AF29" s="2"/>
       <c r="AG29" s="2" t="s">
@@ -3243,10 +3263,10 @@
         <v>80</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>93</v>
@@ -3264,16 +3284,16 @@
         <v>80</v>
       </c>
       <c r="Q30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="S30" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="S30" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="T30" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U30" s="2" t="s">
         <v>93</v>
@@ -3291,10 +3311,10 @@
         <v>80</v>
       </c>
       <c r="AD30" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AE30" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AF30" s="2"/>
       <c r="AG30" s="2" t="s">
@@ -3333,7 +3353,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
@@ -3348,19 +3368,19 @@
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
       <c r="AB31" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
       <c r="AE31" s="2"/>
       <c r="AF31" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AG31" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AH31" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AI31" s="14">
         <v>8</v>
@@ -3397,6 +3417,7 @@
       <c r="C37" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AI31" xr:uid="{333783BD-EC86-4502-A630-819DEFF8253B}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L21 Y2:Y17 C2:C28 L23:L31 Y28:Y31" xr:uid="{864DC9FE-D2BF-46C6-8674-EF3F47262FBF}">
@@ -3414,7 +3435,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H25 U24:U25" xr:uid="{60D55E50-011E-4B72-A099-EBDBD8E688D7}">
       <formula1>"aws-s3,redshift,oracle,mysql,snowflake"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:D27" xr:uid="{BAB4B8B2-7599-4D86-AB86-DA25CCC09125}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:D27 D13" xr:uid="{BAB4B8B2-7599-4D86-AB86-DA25CCC09125}">
       <formula1>"s2tcompare,likeobjectcompare"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U29:U30 H29:H30 H26:H27 U26:U27 H18 U18:U20 H20:H21 U22:U23 H23" xr:uid="{FDFAED56-C639-4DEC-9D7C-4A42D9CC2D05}">
@@ -3438,17 +3459,17 @@
           </x14:formula1>
           <xm:sqref>D2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2153F23C-BB87-46DD-B72C-5F54E9657B4C}">
-          <x14:formula1>
-            <xm:f>config!$C$2:$C$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2 U2</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60062090-6690-4B11-B897-7133E606A12B}">
           <x14:formula1>
             <xm:f>config!$D$2:$D$7</xm:f>
           </x14:formula1>
           <xm:sqref>I2 V2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2153F23C-BB87-46DD-B72C-5F54E9657B4C}">
+          <x14:formula1>
+            <xm:f>config!$E$2:$E$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2 U2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3458,22 +3479,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA0C314-29E7-4BFA-93B1-269ADF583B37}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>44</v>
       </c>
@@ -3481,16 +3503,16 @@
         <v>79</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -3498,16 +3520,16 @@
         <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -3515,61 +3537,82 @@
         <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>87</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>108</v>
-      </c>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>92</v>
-      </c>
+      <c r="E4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>93</v>
-      </c>
+      <c r="E5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>94</v>
-      </c>
+      <c r="E6" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="E7" s="15" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
         <v>97</v>
       </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added the data profiling code
</commit_message>
<xml_diff>
--- a/datf_core/test/testprotocol/traversedtestprotocol.xlsx
+++ b/datf_core/test/testprotocol/traversedtestprotocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venkatesh.thiyag\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966D9D97-CF99-42E6-9577-38CB568969AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0099C2E0-D60F-485F-BE4C-B07B494E253A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1119,7 +1119,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2079,7 +2079,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
updated csv to parquet
</commit_message>
<xml_diff>
--- a/datf_core/test/testprotocol/traversedtestprotocol.xlsx
+++ b/datf_core/test/testprotocol/traversedtestprotocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\DATF_Other\Pyspark\QE_ATF\datf_core\test\testprotocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA217F8-FF49-494C-94A5-F89C4CA228C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0A4370-1F48-4D68-BE7E-B17FC434B1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="184">
   <si>
     <t>Sno.</t>
   </si>
@@ -544,9 +544,6 @@
     <t>test/sql/targetsql</t>
   </si>
   <si>
-    <t>test/data/stage</t>
-  </si>
-  <si>
     <t>test/data/target</t>
   </si>
   <si>
@@ -577,9 +574,6 @@
     <t>dataprofilelimit</t>
   </si>
   <si>
-    <t>testcase31_snowflake_csv_validation</t>
-  </si>
-  <si>
     <t>rtpcr_source</t>
   </si>
   <si>
@@ -589,10 +583,16 @@
     <t>rtpcr_diagnostic_lab_testing</t>
   </si>
   <si>
-    <t>id,state_name</t>
-  </si>
-  <si>
-    <t>test/s2t/s2t_31_snowflake_csv.xlsx</t>
+    <t>testcase31_snowflake_parquet_validation</t>
+  </si>
+  <si>
+    <t>id,state</t>
+  </si>
+  <si>
+    <t>db2</t>
+  </si>
+  <si>
+    <t>test/s2t/s2t_31_snowflake_parquet_val.xlsx</t>
   </si>
 </sst>
 </file>
@@ -780,7 +780,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BAE0998F-A220-496F-A9F2-1D79AF152730}" name="Table1" displayName="Table1" ref="A1:E13" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BAE0998F-A220-496F-A9F2-1D79AF152730}" name="Table1" displayName="Table1" ref="A1:E14" totalsRowShown="0" headerRowDxfId="0">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B7EB12A5-7DBB-4555-B2C0-33C41BB1C784}" name="comparetype"/>
     <tableColumn id="2" xr3:uid="{29FBA9CE-F214-413F-8067-886B551BF267}" name="querygenerationmode"/>
@@ -1126,9 +1126,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333783BD-EC86-4502-A630-819DEFF8253B}">
   <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AG34" sqref="AG34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,7 +1278,7 @@
         <v>75</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -2738,7 +2738,7 @@
         <v>148</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>149</v>
@@ -2783,7 +2783,7 @@
       <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
       <c r="AF22" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AG22" s="2" t="s">
         <v>78</v>
@@ -3194,7 +3194,7 @@
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
       <c r="AF27" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AG27" s="2" t="s">
         <v>78</v>
@@ -3256,7 +3256,7 @@
       <c r="AD28" s="2"/>
       <c r="AE28" s="2"/>
       <c r="AF28" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AG28" s="2" t="s">
         <v>78</v>
@@ -3486,7 +3486,7 @@
       <c r="AD31" s="2"/>
       <c r="AE31" s="2"/>
       <c r="AF31" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AG31" s="2" t="s">
         <v>78</v>
@@ -3506,7 +3506,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>31</v>
@@ -3518,7 +3518,7 @@
         <v>77</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>102</v>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
@@ -3541,31 +3541,24 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
       <c r="S32" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="T32" s="2"/>
       <c r="U32" s="2" t="s">
         <v>84</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>148</v>
+        <v>89</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X32" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z32" s="2" t="s">
-        <v>139</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
-      <c r="AB32" s="2" t="s">
-        <v>104</v>
-      </c>
+      <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
       <c r="AD32" s="2"/>
       <c r="AE32" s="2"/>
@@ -3576,7 +3569,7 @@
         <v>78</v>
       </c>
       <c r="AH32" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AI32" s="14">
         <v>5</v>
@@ -3788,7 +3781,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H17 U3:U17 H31 U31 H28 U28 H24 H19" xr:uid="{3EA29DA5-B24B-4A2B-9AC1-8BA4A560D50C}">
       <formula1>"aws-s3,redshift,oracle"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I13 V3:V32 I16:I32" xr:uid="{8F7EDE14-A18F-40DD-B09A-2EC9280539EB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I13 I16:I32 V3:V32" xr:uid="{8F7EDE14-A18F-40DD-B09A-2EC9280539EB}">
       <formula1>"avro,json,parquet,delimitedfile,delta,table"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H25 U24:U25 H32" xr:uid="{60D55E50-011E-4B72-A099-EBDBD8E688D7}">
@@ -3841,7 +3834,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3910,7 +3903,7 @@
         <v>88</v>
       </c>
       <c r="E4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3918,7 +3911,7 @@
         <v>89</v>
       </c>
       <c r="E5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3959,12 +3952,17 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>176</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
native query generation fixed
</commit_message>
<xml_diff>
--- a/datf_core/test/testprotocol/traversedtestprotocol.xlsx
+++ b/datf_core/test/testprotocol/traversedtestprotocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\DATF_Other\Pyspark\QE_ATF\datf_core\test\testprotocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAE14F9-004D-4C21-B1A8-5A9F99C111B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8596C40A-BB30-4407-AF45-292A901B5282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="187">
   <si>
     <t>Sno.</t>
   </si>
@@ -508,9 +508,6 @@
     <t>test/s2t/source_parquet_target_parquet_s2t_1.xlsx</t>
   </si>
   <si>
-    <t>test/s2t/source_parquet_target_parquet_s2t_2.xlsx</t>
-  </si>
-  <si>
     <t>test/s2t/source_csv_target_csv_s2t_3.xlsx</t>
   </si>
   <si>
@@ -532,9 +529,6 @@
     <t>test/s2t/source_json_target_parquet_s2t_9_match.xlsx</t>
   </si>
   <si>
-    <t>test/s2t/source_json_target_parquet_s2t_10_mismatch.xlsx</t>
-  </si>
-  <si>
     <t>test/data/source</t>
   </si>
   <si>
@@ -593,6 +587,21 @@
   </si>
   <si>
     <t>test/s2t/s2t_31_snowflake_parquet_val.xlsx</t>
+  </si>
+  <si>
+    <t>test/s2t/s2t_10_json_parquet_match.xlsx</t>
+  </si>
+  <si>
+    <t>test/s2t/s2t_5_csv_parquet_match.xlsx</t>
+  </si>
+  <si>
+    <t>test/s2t/s2t_6_csv_parquet_mismatch.xlsx</t>
+  </si>
+  <si>
+    <t>test/s2t/s2t_1_parquet_parquet_mismatch.xlsx</t>
+  </si>
+  <si>
+    <t>test/s2t/s2t_2_parquet_parquet_match.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1126,9 +1135,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333783BD-EC86-4502-A630-819DEFF8253B}">
   <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ32" sqref="AJ32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,7 +1287,7 @@
         <v>75</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -1324,12 +1333,14 @@
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2" t="s">
-        <v>154</v>
+        <v>185</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AH2" s="2"/>
+      <c r="AH2" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="AI2" s="2">
         <v>5</v>
       </c>
@@ -1380,12 +1391,14 @@
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2" t="s">
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="AG3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AH3" s="2"/>
+      <c r="AH3" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="AI3" s="2">
         <v>5</v>
       </c>
@@ -1436,12 +1449,14 @@
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
       <c r="AF4" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AG4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AH4" s="2"/>
+      <c r="AH4" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="AI4" s="2">
         <v>5</v>
       </c>
@@ -1492,12 +1507,14 @@
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AG5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AH5" s="2"/>
+      <c r="AH5" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="AI5" s="2">
         <v>5</v>
       </c>
@@ -1548,12 +1565,14 @@
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="AG6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AH6" s="2"/>
+      <c r="AH6" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="AI6" s="2">
         <v>5</v>
       </c>
@@ -1604,12 +1623,14 @@
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="2" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="AG7" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AH7" s="2"/>
+      <c r="AH7" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="AI7" s="2">
         <v>5</v>
       </c>
@@ -1660,12 +1681,14 @@
       <c r="AD8" s="2"/>
       <c r="AE8" s="2"/>
       <c r="AF8" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AH8" s="2"/>
+      <c r="AH8" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="AI8" s="2">
         <v>5</v>
       </c>
@@ -1716,12 +1739,14 @@
       <c r="AD9" s="2"/>
       <c r="AE9" s="2"/>
       <c r="AF9" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AG9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AH9" s="2"/>
+      <c r="AH9" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="AI9" s="2">
         <v>5</v>
       </c>
@@ -1772,7 +1797,7 @@
       <c r="AD10" s="2"/>
       <c r="AE10" s="2"/>
       <c r="AF10" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG10" s="2" t="s">
         <v>78</v>
@@ -1830,12 +1855,14 @@
       <c r="AD11" s="2"/>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="AG11" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AH11" s="2"/>
+      <c r="AH11" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="AI11" s="2">
         <v>5</v>
       </c>
@@ -1872,7 +1899,7 @@
         <v>89</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>128</v>
@@ -1885,7 +1912,7 @@
         <v>80</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="R12" s="2" t="s">
         <v>133</v>
@@ -1903,7 +1930,7 @@
         <v>89</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="X12" s="2" t="s">
         <v>128</v>
@@ -1916,7 +1943,7 @@
         <v>80</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AE12" s="2" t="s">
         <v>136</v>
@@ -1966,7 +1993,7 @@
         <v>89</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>128</v>
@@ -1979,7 +2006,7 @@
         <v>80</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="R13" s="2" t="s">
         <v>133</v>
@@ -1997,7 +2024,7 @@
         <v>89</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="X13" s="2" t="s">
         <v>128</v>
@@ -2010,7 +2037,7 @@
         <v>80</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AE13" s="2" t="s">
         <v>137</v>
@@ -2058,7 +2085,7 @@
         <v>88</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>138</v>
@@ -2073,7 +2100,7 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="R14" s="2" t="s">
         <v>140</v>
@@ -2091,7 +2118,7 @@
         <v>89</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="X14" s="2" t="s">
         <v>128</v>
@@ -2102,13 +2129,13 @@
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AE14" s="2" t="s">
         <v>136</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AG14" s="2" t="s">
         <v>78</v>
@@ -2152,7 +2179,7 @@
         <v>88</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>138</v>
@@ -2167,7 +2194,7 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="R15" s="2" t="s">
         <v>140</v>
@@ -2185,7 +2212,7 @@
         <v>89</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="X15" s="2" t="s">
         <v>128</v>
@@ -2196,13 +2223,13 @@
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AE15" s="2" t="s">
         <v>137</v>
       </c>
       <c r="AF15" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AG15" s="2" t="s">
         <v>78</v>
@@ -2246,7 +2273,7 @@
         <v>89</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>128</v>
@@ -2271,7 +2298,7 @@
         <v>89</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="X16" s="2" t="s">
         <v>128</v>
@@ -2326,7 +2353,7 @@
         <v>89</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>128</v>
@@ -2351,7 +2378,7 @@
         <v>89</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>141</v>
@@ -2489,7 +2516,7 @@
         <v>89</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>128</v>
@@ -2738,7 +2765,7 @@
         <v>148</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>149</v>
@@ -2783,7 +2810,7 @@
       <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
       <c r="AF22" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AG22" s="2" t="s">
         <v>78</v>
@@ -2910,7 +2937,7 @@
         <v>89</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>128</v>
@@ -3194,7 +3221,7 @@
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
       <c r="AF27" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AG27" s="2" t="s">
         <v>78</v>
@@ -3256,7 +3283,7 @@
       <c r="AD28" s="2"/>
       <c r="AE28" s="2"/>
       <c r="AF28" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AG28" s="2" t="s">
         <v>78</v>
@@ -3309,7 +3336,7 @@
         <v>80</v>
       </c>
       <c r="Q29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="R29" s="2" t="s">
         <v>116</v>
@@ -3336,7 +3363,7 @@
         <v>80</v>
       </c>
       <c r="AD29" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AE29" s="2" t="s">
         <v>118</v>
@@ -3393,7 +3420,7 @@
         <v>80</v>
       </c>
       <c r="Q30" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="R30" s="2" t="s">
         <v>112</v>
@@ -3420,7 +3447,7 @@
         <v>80</v>
       </c>
       <c r="AD30" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AE30" s="2" t="s">
         <v>114</v>
@@ -3486,7 +3513,7 @@
       <c r="AD31" s="2"/>
       <c r="AE31" s="2"/>
       <c r="AF31" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AG31" s="2" t="s">
         <v>78</v>
@@ -3506,7 +3533,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>31</v>
@@ -3518,7 +3545,7 @@
         <v>77</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>102</v>
@@ -3531,7 +3558,7 @@
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
@@ -3541,7 +3568,7 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
       <c r="S32" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="T32" s="2"/>
       <c r="U32" s="2" t="s">
@@ -3551,7 +3578,7 @@
         <v>89</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="X32" s="2" t="s">
         <v>141</v>
@@ -3563,13 +3590,13 @@
       <c r="AD32" s="2"/>
       <c r="AE32" s="2"/>
       <c r="AF32" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AG32" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AH32" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AI32" s="14">
         <v>8</v>
@@ -3903,7 +3930,7 @@
         <v>88</v>
       </c>
       <c r="E4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3911,7 +3938,7 @@
         <v>89</v>
       </c>
       <c r="E5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3952,17 +3979,17 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>